<commit_message>
++ update template import container
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.Documentation/eFMS.API.Documentation/Resources/Files/ContainerImportTemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.Documentation/eFMS.API.Documentation/Resources/Files/ContainerImportTemplate.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\efms\src\WebAPI\eFMS.API.SystemWeb\DocumentationManagement\eFMS.API.Documentation\Resources\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenny.thuong\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
-    <t>Cont Type</t>
-  </si>
-  <si>
-    <t>Cont Qty</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Package Qty</t>
   </si>
   <si>
@@ -84,12 +78,18 @@
   </si>
   <si>
     <t>Commodity</t>
+  </si>
+  <si>
+    <t>Cont Type (*)</t>
+  </si>
+  <si>
+    <t>Cont Qty (*)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,71 +429,71 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="H17" activeCellId="1" sqref="B1 H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" customWidth="1"/>
-    <col min="8" max="8" width="17.54296875" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2">
         <v>12</v>
@@ -508,22 +508,22 @@
         <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -538,7 +538,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -553,7 +553,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -568,7 +568,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -583,7 +583,7 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -598,7 +598,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -613,7 +613,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -628,7 +628,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -643,7 +643,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -658,7 +658,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>

</xml_diff>